<commit_message>
continue to update list of national parks
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAA3315-DB4A-445D-A5E0-90BCF0DFCC11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508AA699-EE35-4F56-A140-440E8EE07020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Park</t>
   </si>
@@ -130,6 +130,93 @@
   </si>
   <si>
     <t>Aztec Ruins National Monument</t>
+  </si>
+  <si>
+    <t>Badlands National Park</t>
+  </si>
+  <si>
+    <t>Baltimore National Heritage Area</t>
+  </si>
+  <si>
+    <t>Baltimore-Washington Parkway</t>
+  </si>
+  <si>
+    <t>Bandelier National Monument</t>
+  </si>
+  <si>
+    <t>Belmont-Paul Women's Equality National Monument</t>
+  </si>
+  <si>
+    <t>Bent's Old Fort National Historic Site</t>
+  </si>
+  <si>
+    <t>Bering Land Bridge National Preserve</t>
+  </si>
+  <si>
+    <t>Big Bend National Park</t>
+  </si>
+  <si>
+    <t>Big Cypress National Preserve</t>
+  </si>
+  <si>
+    <t>Big Hole National Battlefield</t>
+  </si>
+  <si>
+    <t>Big South Fork National River and Recreation Area</t>
+  </si>
+  <si>
+    <t>Big Thicket Nationl Preserve</t>
+  </si>
+  <si>
+    <t>Bighorn Canyon National Recreation Area</t>
+  </si>
+  <si>
+    <t>Birmingham Civil Rights National Monument</t>
+  </si>
+  <si>
+    <t>Biscayne National Park</t>
+  </si>
+  <si>
+    <t>Black Canyon of the Gunnison National Park</t>
+  </si>
+  <si>
+    <t>Blackstone River Valley National Historic Park</t>
+  </si>
+  <si>
+    <t>Blue Ridge National Heritage Area</t>
+  </si>
+  <si>
+    <t>Blue Ridge Parkway</t>
+  </si>
+  <si>
+    <t>Bluestone National Scenic River</t>
+  </si>
+  <si>
+    <t>Booker T Washington National Monument</t>
+  </si>
+  <si>
+    <t>Boston African American National Historic Site</t>
+  </si>
+  <si>
+    <t>Boston Harbor Islands National Recreation Area</t>
+  </si>
+  <si>
+    <t>Boston National Historic Park</t>
+  </si>
+  <si>
+    <t>Brices Cross Roads National Battlefield Site</t>
+  </si>
+  <si>
+    <t>Brown v. Board of Education National Historic Site</t>
+  </si>
+  <si>
+    <t>Bryce Canyon National Park</t>
+  </si>
+  <si>
+    <t>Buck Island Reef National Monument</t>
+  </si>
+  <si>
+    <t>Buffalo National River</t>
   </si>
 </sst>
 </file>
@@ -481,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -656,6 +743,151 @@
         <v>32</v>
       </c>
     </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add parks that start with 'c'
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508AA699-EE35-4F56-A140-440E8EE07020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C533D674-06BE-4191-A815-9B6CEE7F7EC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>Park</t>
   </si>
@@ -217,6 +217,183 @@
   </si>
   <si>
     <t>Buffalo National River</t>
+  </si>
+  <si>
+    <t>Cabrillo National Monument</t>
+  </si>
+  <si>
+    <t>California National Historic Trail</t>
+  </si>
+  <si>
+    <t>Camp Nelson National Monument</t>
+  </si>
+  <si>
+    <t>Canaveral National Seashore</t>
+  </si>
+  <si>
+    <t>Cane River Creole National Historical Park</t>
+  </si>
+  <si>
+    <t>Cane River National Heritage Area</t>
+  </si>
+  <si>
+    <t>Canyon de Chelly National Monument</t>
+  </si>
+  <si>
+    <t>Canyonlands National Park</t>
+  </si>
+  <si>
+    <t>Cape Cod National Seashore</t>
+  </si>
+  <si>
+    <t>Cape Hatteras National Seashore</t>
+  </si>
+  <si>
+    <t>Cape Henry Memorial Part of Colonial National Historical Park</t>
+  </si>
+  <si>
+    <t>Cape Krusenstern National Monument</t>
+  </si>
+  <si>
+    <t>Cape Lookout National Seashore</t>
+  </si>
+  <si>
+    <t>Capitol Hill Parks</t>
+  </si>
+  <si>
+    <t>Capitol Reef National Park</t>
+  </si>
+  <si>
+    <t>Captain John Smith Chesapeake National Historic Trail</t>
+  </si>
+  <si>
+    <t>Capulin Volcano National Monument</t>
+  </si>
+  <si>
+    <t>Carl Sandburg Home National Historic Site</t>
+  </si>
+  <si>
+    <t>Carlsbad Caverns National Park</t>
+  </si>
+  <si>
+    <t>Carter G. Woodson Home National Historic Site</t>
+  </si>
+  <si>
+    <t>Casa Grande Ruins National Monument</t>
+  </si>
+  <si>
+    <t>Castillo de San Marcos National Monument</t>
+  </si>
+  <si>
+    <t>Castle Clinton National Monument</t>
+  </si>
+  <si>
+    <t>Castle Mountains National Monument</t>
+  </si>
+  <si>
+    <t>Catoctin Mountain Park</t>
+  </si>
+  <si>
+    <t>Cedar Breaks National Monument</t>
+  </si>
+  <si>
+    <t>Cedar Creek &amp; Belle Grove National Historical Park</t>
+  </si>
+  <si>
+    <t>Chaco Culture National Historical Park</t>
+  </si>
+  <si>
+    <t>Chamizal National Memorial</t>
+  </si>
+  <si>
+    <t>Champlain Valley National Heritage Partnership</t>
+  </si>
+  <si>
+    <t>Channel Islands National Park</t>
+  </si>
+  <si>
+    <t>Charles Pinckney National Historic Site</t>
+  </si>
+  <si>
+    <t>Charles Young Buffalo Soldiers National Monument</t>
+  </si>
+  <si>
+    <t>Chattahoochee River National Recreation Area</t>
+  </si>
+  <si>
+    <t>Chesapeake &amp; Ohio Canal National Historical Park</t>
+  </si>
+  <si>
+    <t>Chesapeake Bay</t>
+  </si>
+  <si>
+    <t>Chickamauga &amp; Chattanooga National Military Park</t>
+  </si>
+  <si>
+    <t>Chickasaw National Recreation Area</t>
+  </si>
+  <si>
+    <t>Chiricahua National Monument</t>
+  </si>
+  <si>
+    <t>Christiansted National Historic Site</t>
+  </si>
+  <si>
+    <t>City Of Rocks National Reserve</t>
+  </si>
+  <si>
+    <t>Civil War Defenses of Washington</t>
+  </si>
+  <si>
+    <t>Clara Barton National Historic Site</t>
+  </si>
+  <si>
+    <t>Coal National Heritage Area</t>
+  </si>
+  <si>
+    <t>Colonial National Historical Park</t>
+  </si>
+  <si>
+    <t>Colorado National Monument</t>
+  </si>
+  <si>
+    <t>Coltsville National Historical Park</t>
+  </si>
+  <si>
+    <t>Congaree National Park</t>
+  </si>
+  <si>
+    <t>Constitution Gardens</t>
+  </si>
+  <si>
+    <t>Coronado National Memorial</t>
+  </si>
+  <si>
+    <t>Cowpens National Battlefield</t>
+  </si>
+  <si>
+    <t>Crater Lake National Park</t>
+  </si>
+  <si>
+    <t>Craters Of The Moon National Monument &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Crossroads of the American Revolution National Heritage Area</t>
+  </si>
+  <si>
+    <t>Cumberland Gap National Historical Park</t>
+  </si>
+  <si>
+    <t>Cumberland Island National Seashore</t>
+  </si>
+  <si>
+    <t>Curecanti National Recreation Area</t>
+  </si>
+  <si>
+    <t>Cuyahoga Valley National Park</t>
+  </si>
+  <si>
+    <t>César E. Chávez National Monument</t>
   </si>
 </sst>
 </file>
@@ -568,15 +745,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A124" sqref="A124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48" customWidth="1"/>
+    <col min="1" max="1" width="62.26953125" customWidth="1"/>
     <col min="2" max="2" width="42.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -888,6 +1065,301 @@
         <v>61</v>
       </c>
     </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A103" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A104" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A105" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A106" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A107" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A108" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A109" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A110" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A111" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A112" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A113" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A114" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A116" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A117" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A118" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A119" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A120" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A121" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A122" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'e' and 'f' parks
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7A92E21-8E07-4DB2-978D-B226A26EDACB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C357E78-ABDC-4E95-A6A7-6CED22921F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>Park</t>
   </si>
@@ -427,6 +427,168 @@
   </si>
   <si>
     <t>Dry Tortugas National Park</t>
+  </si>
+  <si>
+    <t>Ebey's Landing National Historical Reserve</t>
+  </si>
+  <si>
+    <t>Edgar Allan Poe National Historic Site</t>
+  </si>
+  <si>
+    <t>Effigy Mounds National Monument</t>
+  </si>
+  <si>
+    <t>Eisenhower National Historic Site</t>
+  </si>
+  <si>
+    <t>El Camino Real de los Tejas National Historic Trail</t>
+  </si>
+  <si>
+    <t>El Camino Real de Tierra Adentro National Historic Trail</t>
+  </si>
+  <si>
+    <t>El Malpais National Monument</t>
+  </si>
+  <si>
+    <t>El Morro National Monument</t>
+  </si>
+  <si>
+    <t>Eleanor Roosevelt National Historic Site</t>
+  </si>
+  <si>
+    <t>Ellis Island Part of Statue of Liberty National Monument</t>
+  </si>
+  <si>
+    <t>Erie Canalway National Heritage Corridor</t>
+  </si>
+  <si>
+    <t>Essex National Heritage Area</t>
+  </si>
+  <si>
+    <t>Eugene O'Neill National Historic Site</t>
+  </si>
+  <si>
+    <t>Everglades National Park</t>
+  </si>
+  <si>
+    <t>Fallen Timbers Battlefield and Fort Miamis National Historic Site</t>
+  </si>
+  <si>
+    <t>Federal Hall National Memorial</t>
+  </si>
+  <si>
+    <t>Fire Island National Seashore</t>
+  </si>
+  <si>
+    <t>First Ladies National Historic Site</t>
+  </si>
+  <si>
+    <t>First State National Historical Park</t>
+  </si>
+  <si>
+    <t>Flight 93 National Memorial</t>
+  </si>
+  <si>
+    <t>Florissant Fossil Beds National Monument</t>
+  </si>
+  <si>
+    <t>Ford's Theatre</t>
+  </si>
+  <si>
+    <t>Fort Bowie National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Caroline National Memorial</t>
+  </si>
+  <si>
+    <t>Fort Davis National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Donelson National Battlefield</t>
+  </si>
+  <si>
+    <t>Fort Dupont Park</t>
+  </si>
+  <si>
+    <t>Fort Foote Park</t>
+  </si>
+  <si>
+    <t>Fort Frederica National Monument</t>
+  </si>
+  <si>
+    <t>Fort Laramie National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Larned National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Matanzas National Monument</t>
+  </si>
+  <si>
+    <t>Fort McHenry National Monument and Historic Shrine</t>
+  </si>
+  <si>
+    <t>Fort Monroe National Monument</t>
+  </si>
+  <si>
+    <t>Fort Necessity National Battlefield</t>
+  </si>
+  <si>
+    <t>Fort Point National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Pulaski National Monument</t>
+  </si>
+  <si>
+    <t>Fort Raleigh National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Scott National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Smith National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Stanwix National Monument</t>
+  </si>
+  <si>
+    <t>Fort Sumter and Fort Moultrie National Historical Park</t>
+  </si>
+  <si>
+    <t>Fort Union National Monument</t>
+  </si>
+  <si>
+    <t>Fort Union Trading Post National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Vancouver National Historic Site</t>
+  </si>
+  <si>
+    <t>Fort Washington Park</t>
+  </si>
+  <si>
+    <t>Fossil Butte National Monument</t>
+  </si>
+  <si>
+    <t>Franklin Delano Roosevelt Memorial</t>
+  </si>
+  <si>
+    <t>Frederick Douglass National Historic Site</t>
+  </si>
+  <si>
+    <t>Frederick Law Olmsted National Historic Site</t>
+  </si>
+  <si>
+    <t>Fredericksburg &amp; Spotsylvania National Military Park</t>
+  </si>
+  <si>
+    <t>Freedom Riders National Monument</t>
+  </si>
+  <si>
+    <t>Freedom's Way National Heritage Area</t>
+  </si>
+  <si>
+    <t>Friendship Hill National Historic Site</t>
   </si>
 </sst>
 </file>
@@ -778,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
-  <dimension ref="A1:B134"/>
+  <dimension ref="A1:B190"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
+      <selection activeCell="A190" sqref="A190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,6 +1610,276 @@
         <v>131</v>
       </c>
     </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A136" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A137" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A138" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A139" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A142" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A143" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A144" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A145" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A146" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A147" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A148" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A149" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A151" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A152" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A153" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A154" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A155" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A156" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A157" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A158" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A159" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A160" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A161" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A162" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A163" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A164" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A165" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A166" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A167" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A168" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A169" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A170" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A171" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A172" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A173" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A174" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A175" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A176" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A177" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A178" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A179" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A180" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A181" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A182" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A183" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A184" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A185" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A186" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A187" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A188" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A189" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'g' and 'h' parks
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C357E78-ABDC-4E95-A6A7-6CED22921F09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B836C20F-0897-4A36-8015-B48FC61A095D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
   <si>
     <t>Park</t>
   </si>
@@ -589,6 +589,174 @@
   </si>
   <si>
     <t>Friendship Hill National Historic Site</t>
+  </si>
+  <si>
+    <t>Gates Of The Arctic National Park &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Gateway Arch National Park</t>
+  </si>
+  <si>
+    <t>Gateway National Recreation Area</t>
+  </si>
+  <si>
+    <t>Gauley River National Recreation Area</t>
+  </si>
+  <si>
+    <t>General Grant National Memorial</t>
+  </si>
+  <si>
+    <t>George Rogers Clark National Historical Park</t>
+  </si>
+  <si>
+    <t>George Washington Birthplace National Monument</t>
+  </si>
+  <si>
+    <t>George Washington Carver National Monument</t>
+  </si>
+  <si>
+    <t>George Washington Memorial Parkway</t>
+  </si>
+  <si>
+    <t>Gettysburg National Military Park</t>
+  </si>
+  <si>
+    <t>Gila Cliff Dwellings National Monument</t>
+  </si>
+  <si>
+    <t>Glacier Bay National Park &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Glacier National Park</t>
+  </si>
+  <si>
+    <t>Glen Canyon National Recreation Area</t>
+  </si>
+  <si>
+    <t>Glen Echo Park</t>
+  </si>
+  <si>
+    <t>Gloria Dei Church National Historic Site</t>
+  </si>
+  <si>
+    <t>Golden Gate National Recreation Area</t>
+  </si>
+  <si>
+    <t>Golden Spike National Historical Park</t>
+  </si>
+  <si>
+    <t>Governors Island National Monument</t>
+  </si>
+  <si>
+    <t>Grand Canyon National Park</t>
+  </si>
+  <si>
+    <t>Grand Portage National Monument</t>
+  </si>
+  <si>
+    <t>Grand Teton National Park</t>
+  </si>
+  <si>
+    <t>Grant-Kohrs Ranch National Historic Site</t>
+  </si>
+  <si>
+    <t>Great Basin National Park</t>
+  </si>
+  <si>
+    <t>Great Egg Harbor River</t>
+  </si>
+  <si>
+    <t>Great Falls Park</t>
+  </si>
+  <si>
+    <t>Great Sand Dunes National Park &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Great Smoky Mountains National Park</t>
+  </si>
+  <si>
+    <t>Green Springs</t>
+  </si>
+  <si>
+    <t>Greenbelt Park</t>
+  </si>
+  <si>
+    <t>Guadalupe Mountains National Park</t>
+  </si>
+  <si>
+    <t>Guilford Courthouse National Military Park</t>
+  </si>
+  <si>
+    <t>Gulf Islands National Seashore</t>
+  </si>
+  <si>
+    <t>Gullah/Geechee Cultural Heritage Corridor</t>
+  </si>
+  <si>
+    <t>Hagerman Fossil Beds National Monument</t>
+  </si>
+  <si>
+    <t>Haleakalā National Park</t>
+  </si>
+  <si>
+    <t>Hamilton Grange National Memorial</t>
+  </si>
+  <si>
+    <t>Hampton National Historic Site</t>
+  </si>
+  <si>
+    <t>Harmony Hall</t>
+  </si>
+  <si>
+    <t>Harpers Ferry National Historical Park</t>
+  </si>
+  <si>
+    <t>Harriet Tubman National Historical Park</t>
+  </si>
+  <si>
+    <t>Harriet Tubman Underground Railroad National Historical Park</t>
+  </si>
+  <si>
+    <t>Harry S Truman National Historic Site</t>
+  </si>
+  <si>
+    <t>Hawai'i Volcanoes National Park</t>
+  </si>
+  <si>
+    <t>Herbert Hoover National Historic Site</t>
+  </si>
+  <si>
+    <t>Historic Jamestowne Part of Colonial National Historical Park</t>
+  </si>
+  <si>
+    <t>Home Of Franklin D Roosevelt National Historic Site</t>
+  </si>
+  <si>
+    <t>Homestead National Monument of America</t>
+  </si>
+  <si>
+    <t>Honouliuli National Historic Site</t>
+  </si>
+  <si>
+    <t>Hopewell Culture National Historical Park</t>
+  </si>
+  <si>
+    <t>Hopewell Furnace National Historic Site</t>
+  </si>
+  <si>
+    <t>Horseshoe Bend National Military Park</t>
+  </si>
+  <si>
+    <t>Hot Springs National Park</t>
+  </si>
+  <si>
+    <t>Hovenweep National Monument</t>
+  </si>
+  <si>
+    <t>Hubbell Trading Post National Historic Site</t>
+  </si>
+  <si>
+    <t>Hudson River Valley National Heritage Area</t>
   </si>
 </sst>
 </file>
@@ -940,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
-  <dimension ref="A1:B190"/>
+  <dimension ref="A1:B248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A179" workbookViewId="0">
-      <selection activeCell="A190" sqref="A190"/>
+    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="A248" sqref="A248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1880,6 +2048,286 @@
         <v>185</v>
       </c>
     </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A197" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A199" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A200" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A205" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A206" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A214" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A216" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A217" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A222" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A223" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A230" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A232" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A242" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A243" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>241</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add 'I' through 'N'.
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B836C20F-0897-4A36-8015-B48FC61A095D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D829326-BCF7-4CF6-802C-D4E7C41CDAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="348">
   <si>
     <t>Park</t>
   </si>
@@ -757,6 +757,324 @@
   </si>
   <si>
     <t>Hudson River Valley National Heritage Area</t>
+  </si>
+  <si>
+    <t>Iñupiat Heritage Center</t>
+  </si>
+  <si>
+    <t>Ice Age Floods National Geologic Trail</t>
+  </si>
+  <si>
+    <t>Ice Age National Scenic Trail</t>
+  </si>
+  <si>
+    <t>Independence National Historical Park</t>
+  </si>
+  <si>
+    <t>Indiana Dunes National Park</t>
+  </si>
+  <si>
+    <t>Isle Royale National Park</t>
+  </si>
+  <si>
+    <t>James A Garfield National Historic Site</t>
+  </si>
+  <si>
+    <t>Jean Lafitte National Historical Park and Preserve</t>
+  </si>
+  <si>
+    <t>Jewel Cave National Monument</t>
+  </si>
+  <si>
+    <t>Jimmy Carter National Historic Site</t>
+  </si>
+  <si>
+    <t>John Day Fossil Beds National Monument</t>
+  </si>
+  <si>
+    <t>John Fitzgerald Kennedy National Historic Site</t>
+  </si>
+  <si>
+    <t>John H. Chafee Blackstone River Valley National Heritage Corridor</t>
+  </si>
+  <si>
+    <t>John Muir National Historic Site</t>
+  </si>
+  <si>
+    <t>Johnstown Flood National Memorial</t>
+  </si>
+  <si>
+    <t>Joshua Tree National Park</t>
+  </si>
+  <si>
+    <t>Journey Through Hallowed Ground National Heritage Area</t>
+  </si>
+  <si>
+    <t>Juan Bautista de Anza National Historic Trail</t>
+  </si>
+  <si>
+    <t>Kalaupapa National Historical Park</t>
+  </si>
+  <si>
+    <t>Kaloko-Honokōhau National Historical Park</t>
+  </si>
+  <si>
+    <t>Katahdin Woods and Waters National Monument</t>
+  </si>
+  <si>
+    <t>Katmai National Park &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Kenai Fjords National Park</t>
+  </si>
+  <si>
+    <t>Kenilworth Park &amp; Aquatic Gardens</t>
+  </si>
+  <si>
+    <t>Kennesaw Mountain National Battlefield Park</t>
+  </si>
+  <si>
+    <t>Keweenaw National Historical Park</t>
+  </si>
+  <si>
+    <t>Kings Mountain National Military Park</t>
+  </si>
+  <si>
+    <t>Klondike Gold Rush - Seattle Unit National Historical Park</t>
+  </si>
+  <si>
+    <t>Klondike Gold Rush National Historical Park</t>
+  </si>
+  <si>
+    <t>Knife River Indian Villages National Historic Site</t>
+  </si>
+  <si>
+    <t>Kobuk Valley National Park</t>
+  </si>
+  <si>
+    <t>Korean War Veterans Memorial</t>
+  </si>
+  <si>
+    <t>Lake Clark National Park &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Lake Mead National Recreation Area</t>
+  </si>
+  <si>
+    <t>Lake Meredith National Recreation Area</t>
+  </si>
+  <si>
+    <t>Lake Roosevelt National Recreation Area</t>
+  </si>
+  <si>
+    <t>Lassen Volcanic National Park</t>
+  </si>
+  <si>
+    <t>Lava Beds National Monument</t>
+  </si>
+  <si>
+    <t>LBJ Memorial Grove on the Potomac</t>
+  </si>
+  <si>
+    <t>Lewis &amp; Clark National Historic Trail</t>
+  </si>
+  <si>
+    <t>Lewis and Clark National Historical Park</t>
+  </si>
+  <si>
+    <t>Lincoln Boyhood National Memorial</t>
+  </si>
+  <si>
+    <t>Lincoln Home National Historic Site</t>
+  </si>
+  <si>
+    <t>Lincoln Memorial</t>
+  </si>
+  <si>
+    <t>Little Bighorn Battlefield National Monument</t>
+  </si>
+  <si>
+    <t>Little River Canyon National Preserve</t>
+  </si>
+  <si>
+    <t>Little Rock Central High School National Historic Site</t>
+  </si>
+  <si>
+    <t>Longfellow House Washington's Headquarters National Historic Site</t>
+  </si>
+  <si>
+    <t>Lowell National Historical Park</t>
+  </si>
+  <si>
+    <t>Lower Delaware National Wild and Scenic River</t>
+  </si>
+  <si>
+    <t>Lower East Side Tenement Museum National Historic Site</t>
+  </si>
+  <si>
+    <t>Lyndon B Johnson National Historical Park</t>
+  </si>
+  <si>
+    <t>Maggie L Walker National Historic Site</t>
+  </si>
+  <si>
+    <t>Maine Acadian Culture</t>
+  </si>
+  <si>
+    <t>Mammoth Cave National Park</t>
+  </si>
+  <si>
+    <t>Manassas National Battlefield Park</t>
+  </si>
+  <si>
+    <t>Manhattan Project National Historical Park</t>
+  </si>
+  <si>
+    <t>Manzanar National Historic Site</t>
+  </si>
+  <si>
+    <t>Marsh - Billings - Rockefeller National Historical Park</t>
+  </si>
+  <si>
+    <t>Martin Luther King, Jr. Memorial</t>
+  </si>
+  <si>
+    <t>Martin Luther King, Jr. National Historical Park</t>
+  </si>
+  <si>
+    <t>Martin Van Buren National Historic Site</t>
+  </si>
+  <si>
+    <t>Mary McLeod Bethune Council House National Historic Site</t>
+  </si>
+  <si>
+    <t>Mesa Verde National Park</t>
+  </si>
+  <si>
+    <t>Minidoka National Historic Site</t>
+  </si>
+  <si>
+    <t>Minute Man National Historical Park</t>
+  </si>
+  <si>
+    <t>Minuteman Missile National Historic Site</t>
+  </si>
+  <si>
+    <t>Mississippi Delta National Heritage Area</t>
+  </si>
+  <si>
+    <t>Mississippi Gulf National Heritage Area</t>
+  </si>
+  <si>
+    <t>Mississippi Hills National Heritage Area</t>
+  </si>
+  <si>
+    <t>Mississippi National River and Recreation Area</t>
+  </si>
+  <si>
+    <t>Missouri National Recreational River</t>
+  </si>
+  <si>
+    <t>Mojave National Preserve</t>
+  </si>
+  <si>
+    <t>Monocacy National Battlefield</t>
+  </si>
+  <si>
+    <t>Montezuma Castle National Monument</t>
+  </si>
+  <si>
+    <t>Moores Creek National Battlefield</t>
+  </si>
+  <si>
+    <t>Mormon Pioneer National Historic Trail</t>
+  </si>
+  <si>
+    <t>Morristown National Historical Park</t>
+  </si>
+  <si>
+    <t>Motor Cities National Heritage Area</t>
+  </si>
+  <si>
+    <t>Mount Rainier National Park</t>
+  </si>
+  <si>
+    <t>Mount Rushmore National Memorial</t>
+  </si>
+  <si>
+    <t>Muir Woods National Monument</t>
+  </si>
+  <si>
+    <t>Muscle Shoals National Heritage Area</t>
+  </si>
+  <si>
+    <t>Natchez National Historical Park</t>
+  </si>
+  <si>
+    <t>Natchez Trace National Scenic Trail</t>
+  </si>
+  <si>
+    <t>Natchez Trace Parkway</t>
+  </si>
+  <si>
+    <t>National Aviation Heritage Area</t>
+  </si>
+  <si>
+    <t>National Capital Parks-East</t>
+  </si>
+  <si>
+    <t>National Mall and Memorial Parks</t>
+  </si>
+  <si>
+    <t>National Park of American Samoa</t>
+  </si>
+  <si>
+    <t>National Parks of New York Harbor</t>
+  </si>
+  <si>
+    <t>Natural Bridges National Monument</t>
+  </si>
+  <si>
+    <t>Navajo National Monument</t>
+  </si>
+  <si>
+    <t>New Bedford Whaling National Historical Park</t>
+  </si>
+  <si>
+    <t>New England National Scenic Trail</t>
+  </si>
+  <si>
+    <t>New Jersey Pinelands National Reserve</t>
+  </si>
+  <si>
+    <t>New Orleans Jazz National Historical Park</t>
+  </si>
+  <si>
+    <t>New River Gorge National River</t>
+  </si>
+  <si>
+    <t>Nez Perce National Historical Park</t>
+  </si>
+  <si>
+    <t>Niagara Falls National Heritage Area</t>
+  </si>
+  <si>
+    <t>Nicodemus National Historic Site</t>
+  </si>
+  <si>
+    <t>Ninety Six National Historic Site</t>
+  </si>
+  <si>
+    <t>Niobrara National Scenic River</t>
+  </si>
+  <si>
+    <t>Noatak National Preserve</t>
+  </si>
+  <si>
+    <t>North Cascades National Park</t>
+  </si>
+  <si>
+    <t>North Country National Scenic Trail</t>
   </si>
 </sst>
 </file>
@@ -1108,10 +1426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
-  <dimension ref="A1:B248"/>
+  <dimension ref="A1:B360"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="A248" sqref="A248"/>
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="A360" sqref="A360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2328,6 +2646,536 @@
         <v>241</v>
       </c>
     </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A250" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A252" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A261" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A262" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A270" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A272" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A273" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A278" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A279" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A286" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A288" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A297" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A298" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A306" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A308" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A309" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A340" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
+        <v>347</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add O-Z to spreadsheet
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D829326-BCF7-4CF6-802C-D4E7C41CDAC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DB1259-AC32-4871-B850-FB19A240E1C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="499">
   <si>
     <t>Park</t>
   </si>
@@ -1075,6 +1075,459 @@
   </si>
   <si>
     <t>North Country National Scenic Trail</t>
+  </si>
+  <si>
+    <t>Obed Wild &amp; Scenic River</t>
+  </si>
+  <si>
+    <t>Ocmulgee Mounds National Historical Park</t>
+  </si>
+  <si>
+    <t>Oil Region National Heritage Area</t>
+  </si>
+  <si>
+    <t>Oklahoma City National Memorial</t>
+  </si>
+  <si>
+    <t>Old Spanish National Historic Trail</t>
+  </si>
+  <si>
+    <t>Olympic National Park</t>
+  </si>
+  <si>
+    <t>Oregon Caves National Monument &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Oregon National Historic Trail</t>
+  </si>
+  <si>
+    <t>Organ Pipe Cactus National Monument</t>
+  </si>
+  <si>
+    <t>Overmountain Victory National Historic Trail</t>
+  </si>
+  <si>
+    <t>Oxon Cove  Park &amp; Oxon Hill Farm</t>
+  </si>
+  <si>
+    <t>Ozark National Scenic Riverways</t>
+  </si>
+  <si>
+    <t>Padre Island National Seashore</t>
+  </si>
+  <si>
+    <t>Palo Alto Battlefield National Historical Park</t>
+  </si>
+  <si>
+    <t>Parashant National Monument</t>
+  </si>
+  <si>
+    <t>Paterson Great Falls National Historical Park</t>
+  </si>
+  <si>
+    <t>Pea Ridge National Military Park</t>
+  </si>
+  <si>
+    <t>Pearl Harbor National Memorial</t>
+  </si>
+  <si>
+    <t>Pecos National Historical Park</t>
+  </si>
+  <si>
+    <t>Pennsylvania Avenue</t>
+  </si>
+  <si>
+    <t>Perry's Victory &amp; International Peace Memorial</t>
+  </si>
+  <si>
+    <t>Petersburg National Battlefield</t>
+  </si>
+  <si>
+    <t>Petrified Forest National Park</t>
+  </si>
+  <si>
+    <t>Petroglyph National Monument</t>
+  </si>
+  <si>
+    <t>Pictured Rocks National Lakeshore</t>
+  </si>
+  <si>
+    <t>Pinnacles National Park</t>
+  </si>
+  <si>
+    <t>Pipe Spring National Monument</t>
+  </si>
+  <si>
+    <t>Pipestone National Monument</t>
+  </si>
+  <si>
+    <t>Piscataway Park</t>
+  </si>
+  <si>
+    <t>Point Reyes National Seashore</t>
+  </si>
+  <si>
+    <t>Pony Express National Historic Trail</t>
+  </si>
+  <si>
+    <t>Port Chicago Naval Magazine National Memorial</t>
+  </si>
+  <si>
+    <t>Potomac Heritage National Scenic Trail</t>
+  </si>
+  <si>
+    <t>Poverty Point National Monument</t>
+  </si>
+  <si>
+    <t>President William Jefferson Clinton Birthplace Home National Historic Site</t>
+  </si>
+  <si>
+    <t>President's Park</t>
+  </si>
+  <si>
+    <t>Presidio of San Francisco</t>
+  </si>
+  <si>
+    <t>Prince William Forest Park</t>
+  </si>
+  <si>
+    <t>Pu`uhonua O Hōnaunau National Historical Park</t>
+  </si>
+  <si>
+    <t>Pu`ukoholā Heiau National Historic Site</t>
+  </si>
+  <si>
+    <t>Pullman National Monument</t>
+  </si>
+  <si>
+    <t>Rainbow Bridge National Monument</t>
+  </si>
+  <si>
+    <t>Reconstruction Era National Historical Park</t>
+  </si>
+  <si>
+    <t>Redwood National and State Parks</t>
+  </si>
+  <si>
+    <t>Richmond National Battlefield Park</t>
+  </si>
+  <si>
+    <t>Rio Grande Wild &amp; Scenic River</t>
+  </si>
+  <si>
+    <t>River Raisin National Battlefield Park</t>
+  </si>
+  <si>
+    <t>Rivers Of Steel National Heritage Area</t>
+  </si>
+  <si>
+    <t>Rock Creek Park</t>
+  </si>
+  <si>
+    <t>Rocky Mountain National Park</t>
+  </si>
+  <si>
+    <t>Roger Williams National Memorial</t>
+  </si>
+  <si>
+    <t>Roosevelt Campobello International Park</t>
+  </si>
+  <si>
+    <t>Rosie the Riveter WWII Home Front National Historical Park</t>
+  </si>
+  <si>
+    <t>Russell Cave National Monument</t>
+  </si>
+  <si>
+    <t>Sagamore Hill National Historic Site</t>
+  </si>
+  <si>
+    <t>Saguaro National Park</t>
+  </si>
+  <si>
+    <t>Saint Croix Island International Historic Site</t>
+  </si>
+  <si>
+    <t>Saint Croix National Scenic Riverway</t>
+  </si>
+  <si>
+    <t>Saint Paul's Church National Historic Site</t>
+  </si>
+  <si>
+    <t>Saint-Gaudens National Historical Park</t>
+  </si>
+  <si>
+    <t>Salem Maritime National Historic Site</t>
+  </si>
+  <si>
+    <t>Salinas Pueblo Missions National Monument</t>
+  </si>
+  <si>
+    <t>Salt River Bay National Historical Park and Ecological Preserve</t>
+  </si>
+  <si>
+    <t>San Antonio Missions National Historical Park</t>
+  </si>
+  <si>
+    <t>San Francisco Maritime National Historical Park</t>
+  </si>
+  <si>
+    <t>San Juan Island National Historical Park</t>
+  </si>
+  <si>
+    <t>San Juan National Historic Site</t>
+  </si>
+  <si>
+    <t>Sand Creek Massacre National Historic Site</t>
+  </si>
+  <si>
+    <t>Santa Fe National Historic Trail</t>
+  </si>
+  <si>
+    <t>Santa Monica Mountains National Recreation Area</t>
+  </si>
+  <si>
+    <t>Saratoga National Historical Park</t>
+  </si>
+  <si>
+    <t>Saugus Iron Works National Historic Site</t>
+  </si>
+  <si>
+    <t>Schuylkill River Valley National Heritage Area</t>
+  </si>
+  <si>
+    <t>Scotts Bluff National Monument</t>
+  </si>
+  <si>
+    <t>Selma To Montgomery National Historic Trail</t>
+  </si>
+  <si>
+    <t>Sequoia &amp; Kings Canyon National Parks</t>
+  </si>
+  <si>
+    <t>Shenandoah National Park</t>
+  </si>
+  <si>
+    <t>Shenandoah Valley Battlefields National Historic District</t>
+  </si>
+  <si>
+    <t>Shiloh National Military Park</t>
+  </si>
+  <si>
+    <t>Sitka National Historical Park</t>
+  </si>
+  <si>
+    <t>Sleeping Bear Dunes National Lakeshore</t>
+  </si>
+  <si>
+    <t>South Carolina National Heritage Corridor</t>
+  </si>
+  <si>
+    <t>Springfield Armory National Historic Site</t>
+  </si>
+  <si>
+    <t>Star-Spangled Banner National Historic Trail</t>
+  </si>
+  <si>
+    <t>Statue Of Liberty National Monument</t>
+  </si>
+  <si>
+    <t>Steamtown National Historic Site</t>
+  </si>
+  <si>
+    <t>Stones River National Battlefield</t>
+  </si>
+  <si>
+    <t>Stonewall National Monument</t>
+  </si>
+  <si>
+    <t>Sunset Crater Volcano National Monument</t>
+  </si>
+  <si>
+    <t>Tallgrass Prairie National Preserve</t>
+  </si>
+  <si>
+    <t>Tennessee Civil War National Heritage Area</t>
+  </si>
+  <si>
+    <t>Thaddeus Kosciuszko National Memorial</t>
+  </si>
+  <si>
+    <t>The Last Green Valley National Heritage Corridor</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt Birthplace National Historic Site</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt Inaugural National Historic Site</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt Island</t>
+  </si>
+  <si>
+    <t>Theodore Roosevelt National Park</t>
+  </si>
+  <si>
+    <t>Thomas Cole National Historic Site</t>
+  </si>
+  <si>
+    <t>Thomas Edison National Historical Park</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson Memorial</t>
+  </si>
+  <si>
+    <t>Thomas Stone National Historic Site</t>
+  </si>
+  <si>
+    <t>Timpanogos Cave National Monument</t>
+  </si>
+  <si>
+    <t>Timucuan Ecological &amp; Historic Preserve</t>
+  </si>
+  <si>
+    <t>Tonto National Monument</t>
+  </si>
+  <si>
+    <t>Touro Synagogue National Historic Site</t>
+  </si>
+  <si>
+    <t>Trail Of Tears National Historic Trail</t>
+  </si>
+  <si>
+    <t>Tule Lake National Monument</t>
+  </si>
+  <si>
+    <t>Tule Springs Fossil Beds National Monument</t>
+  </si>
+  <si>
+    <t>Tumacácori National Historical Park</t>
+  </si>
+  <si>
+    <t>Tupelo National Battlefield</t>
+  </si>
+  <si>
+    <t>Tuskegee Airmen National Historic Site</t>
+  </si>
+  <si>
+    <t>Tuskegee Institute National Historic Site</t>
+  </si>
+  <si>
+    <t>Tuzigoot National Monument</t>
+  </si>
+  <si>
+    <t>Ulysses S Grant National Historic Site</t>
+  </si>
+  <si>
+    <t>Upper Delaware Scenic &amp; Recreational River</t>
+  </si>
+  <si>
+    <t>Upper Housatonic Valley National Heritage Area</t>
+  </si>
+  <si>
+    <t>Valles Caldera National Preserve</t>
+  </si>
+  <si>
+    <t>Valley Forge National Historical Park</t>
+  </si>
+  <si>
+    <t>Vanderbilt Mansion National Historic Site</t>
+  </si>
+  <si>
+    <t>Vicksburg National Military Park</t>
+  </si>
+  <si>
+    <t>Vietnam Veterans Memorial</t>
+  </si>
+  <si>
+    <t>Virgin Islands Coral Reef National Monument</t>
+  </si>
+  <si>
+    <t>Virgin Islands National Park</t>
+  </si>
+  <si>
+    <t>Voyageurs National Park</t>
+  </si>
+  <si>
+    <t>Waco Mammoth National Monument</t>
+  </si>
+  <si>
+    <t>Walnut Canyon National Monument</t>
+  </si>
+  <si>
+    <t>War In The Pacific National Historical Park</t>
+  </si>
+  <si>
+    <t>Washington Monument</t>
+  </si>
+  <si>
+    <t>Washington-Rochambeau Revolutionary Route National Historic Trail</t>
+  </si>
+  <si>
+    <t>Washita Battlefield National Historic Site</t>
+  </si>
+  <si>
+    <t>Weir Farm National Historic Site</t>
+  </si>
+  <si>
+    <t>Wheeling National Heritage Area</t>
+  </si>
+  <si>
+    <t>Whiskeytown National Recreation Area</t>
+  </si>
+  <si>
+    <t>White Sands National Monument</t>
+  </si>
+  <si>
+    <t>Whitman Mission National Historic Site</t>
+  </si>
+  <si>
+    <t>William Howard Taft National Historic Site</t>
+  </si>
+  <si>
+    <t>Wilson's Creek National Battlefield</t>
+  </si>
+  <si>
+    <t>Wind Cave National Park</t>
+  </si>
+  <si>
+    <t>Wing Luke Museum Affiliated Area</t>
+  </si>
+  <si>
+    <t>Wolf Trap National Park for the Performing Arts</t>
+  </si>
+  <si>
+    <t>Women's Rights National Historical Park</t>
+  </si>
+  <si>
+    <t>World War II Memorial</t>
+  </si>
+  <si>
+    <t>Wrangell - St Elias National Park &amp; Preserve</t>
+  </si>
+  <si>
+    <t>Wright Brothers National Memorial</t>
+  </si>
+  <si>
+    <t>Wupatki National Monument</t>
+  </si>
+  <si>
+    <t>Yellowstone National Park</t>
+  </si>
+  <si>
+    <t>Yorktown Battlefield Part of Colonial National Historical Park</t>
+  </si>
+  <si>
+    <t>Yosemite National Park</t>
+  </si>
+  <si>
+    <t>Yucca House National Monument</t>
+  </si>
+  <si>
+    <t>Yukon - Charley Rivers National Preserve</t>
+  </si>
+  <si>
+    <t>Zion National Park</t>
   </si>
 </sst>
 </file>
@@ -1426,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
-  <dimension ref="A1:B360"/>
+  <dimension ref="A1:B521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="A360" sqref="A360"/>
+    <sheetView tabSelected="1" topLeftCell="A506" workbookViewId="0">
+      <selection activeCell="A520" sqref="A520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3176,6 +3629,761 @@
         <v>347</v>
       </c>
     </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A363" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A364" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A365" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A368" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A370" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A372" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A373" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A375" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A376" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A377" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A378" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A379" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A380" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A381" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A382" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A383" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A384" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A385" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A386" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A387" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A388" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A389" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A390" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A391" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A392" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A393" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A394" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A395" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A396" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A397" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A398" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A399" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A400" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A401" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A402" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A403" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A405" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A406" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A407" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A408" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A409" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A410" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A411" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A412" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A413" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A414" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A415" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A416" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A417" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A419" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A420" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A421" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A422" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A423" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A424" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A425" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A426" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A427" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A428" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A429" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A430" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A431" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A432" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A433" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A434" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A435" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A436" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A437" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A438" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A439" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A440" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A441" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A442" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A443" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A444" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A445" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A446" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A447" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A448" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A449" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A450" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A451" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A452" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A453" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A455" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A456" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A457" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A458" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A459" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A460" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A461" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A462" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A463" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A464" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A465" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A466" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A467" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A468" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A469" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A470" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A471" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A472" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A473" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A474" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A475" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A476" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A477" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A478" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A480" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A481" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A482" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A484" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A485" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A486" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A487" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A488" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A489" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A490" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A491" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A493" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A494" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A495" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A496" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A497" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A498" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A499" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A500" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A501" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A502" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A503" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A504" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A505" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A506" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A507" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A508" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A509" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A510" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A511" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A512" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A513" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A515" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A516" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A517" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A518" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A519" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A521" t="s">
+        <v>498</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add codes to some parks
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DB1259-AC32-4871-B850-FB19A240E1C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87BB09C-26E4-4F93-9474-5009A9408F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="501">
   <si>
     <t>Park</t>
   </si>
@@ -1528,19 +1528,30 @@
   </si>
   <si>
     <t>Zion National Park</t>
+  </si>
+  <si>
+    <t>c6bca771_1579292693</t>
+  </si>
+  <si>
+    <t>50cfe230_1579293158</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1563,8 +1574,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1881,13 +1896,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{004521FA-64D3-4B03-A7F8-6DCA944E857D}">
   <dimension ref="A1:B521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A506" workbookViewId="0">
-      <selection activeCell="A520" sqref="A520"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="62.26953125" customWidth="1"/>
+    <col min="1" max="1" width="64.453125" customWidth="1"/>
     <col min="2" max="2" width="42.36328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1903,21 +1918,29 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -4386,5 +4409,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Adams Nat Hist Park to Alaska Public Lands to parks object and to excel spreadsheet
</commit_message>
<xml_diff>
--- a/Park Codes.xlsx
+++ b/Park Codes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RateYourNPSseason\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87BB09C-26E4-4F93-9474-5009A9408F7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D388D3-25EF-47CC-8BDF-BC83C66C2584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AABA3781-3792-426D-B1CF-51D8FE5FE464}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="508">
   <si>
     <t>Park</t>
   </si>
@@ -1534,6 +1534,27 @@
   </si>
   <si>
     <t>50cfe230_1579293158</t>
+  </si>
+  <si>
+    <t>3d5933d6_1579294968</t>
+  </si>
+  <si>
+    <t>e10f729b_1579295063</t>
+  </si>
+  <si>
+    <t>cb501ffe_1579295141</t>
+  </si>
+  <si>
+    <t>e328e097_1579295222</t>
+  </si>
+  <si>
+    <t>59c67b4d_1579295281</t>
+  </si>
+  <si>
+    <t>d6d421a0_1579295352</t>
+  </si>
+  <si>
+    <t>2e9e03f5_1579295416</t>
   </si>
 </sst>
 </file>
@@ -1897,7 +1918,7 @@
   <dimension ref="A1:B521"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1934,37 +1955,56 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>